<commit_message>
[RF Gen] 부품 입고 check 및 제작
</commit_message>
<xml_diff>
--- a/0_Block Diagram/Plasma_Gen_Block Diagram.xlsx
+++ b/0_Block Diagram/Plasma_Gen_Block Diagram.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="35">
   <si>
     <t>HD1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,6 +143,18 @@
   </si>
   <si>
     <t>CN3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF_CON_SW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOP_CASE_SW</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -405,15 +417,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -424,22 +427,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -658,8 +670,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>266701</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -670,8 +682,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5591176" y="209550"/>
-          <a:ext cx="4086225" cy="9848850"/>
+          <a:off x="5419726" y="209550"/>
+          <a:ext cx="5476874" cy="9896475"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -712,16 +724,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -730,7 +742,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3800475" y="4162425"/>
+          <a:off x="3476625" y="7639050"/>
           <a:ext cx="1181100" cy="809625"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -832,15 +844,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -849,8 +861,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="8401050"/>
-          <a:ext cx="1181100" cy="809625"/>
+          <a:off x="4086225" y="8534400"/>
+          <a:ext cx="1162050" cy="809625"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -921,6 +933,408 @@
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="모서리가 둥근 직사각형 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7696200" y="7115175"/>
+          <a:ext cx="1123950" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>DC/DC</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>12V -&gt; 5V</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>NCP3064 1.5A</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7591424" y="8239125"/>
+          <a:ext cx="1752601" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>DC/DC</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>5V -&gt; 3.3V</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>LM1117-3.3V 1A</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="모서리가 둥근 직사각형 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11325225" y="3905250"/>
+          <a:ext cx="1162050" cy="809625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Limit S/W</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="모서리가 둥근 직사각형 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11315700" y="4953000"/>
+          <a:ext cx="1162050" cy="809625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Limit S/W</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="오른쪽 화살표 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10782300" y="4229100"/>
+          <a:ext cx="476250" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="오른쪽 화살표 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10782300" y="5295900"/>
+          <a:ext cx="476250" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1216,65 +1630,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:L43"/>
+  <dimension ref="C4:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R35" sqref="R35:R36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="5.75" customWidth="1"/>
+    <col min="3" max="3" width="4.625" customWidth="1"/>
     <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.75" customWidth="1"/>
+    <col min="5" max="5" width="4.625" customWidth="1"/>
     <col min="6" max="6" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.625" customWidth="1"/>
     <col min="10" max="10" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.625" customWidth="1"/>
     <col min="12" max="12" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.625" customWidth="1"/>
+    <col min="15" max="15" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-      <c r="I5" s="3" t="s">
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
+      <c r="I5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="5"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="19"/>
     </row>
     <row r="6" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C6" s="6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="8">
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
         <v>2</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="6">
-        <v>1</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" s="8">
+      <c r="F6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="5">
         <v>2</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C7" s="10">
+      <c r="C7" s="7">
         <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1283,10 +1701,10 @@
       <c r="E7" s="1">
         <v>4</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="10">
+      <c r="F7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="7">
         <v>3</v>
       </c>
       <c r="J7" s="2" t="s">
@@ -1295,12 +1713,12 @@
       <c r="K7" s="1">
         <v>4</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1309,10 +1727,10 @@
       <c r="E8" s="1">
         <v>6</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="7">
         <v>5</v>
       </c>
       <c r="J8" s="2" t="s">
@@ -1321,12 +1739,12 @@
       <c r="K8" s="1">
         <v>6</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="L8" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C9" s="10">
+      <c r="C9" s="7">
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1335,10 +1753,10 @@
       <c r="E9" s="1">
         <v>8</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="10">
+      <c r="F9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="7">
         <v>7</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -1347,79 +1765,79 @@
       <c r="K9" s="1">
         <v>8</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="13">
+      <c r="C10" s="10">
         <v>9</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="14">
+      <c r="D10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="11">
         <v>10</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10" s="13">
+      <c r="F10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="10">
         <v>9</v>
       </c>
-      <c r="J10" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="14">
+      <c r="J10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="11">
         <v>10</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
-      <c r="I12" s="3" t="s">
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="19"/>
+      <c r="I12" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="5"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="19"/>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C13" s="6">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="5">
         <v>2</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="6">
-        <v>1</v>
-      </c>
-      <c r="J13" s="7" t="s">
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="5">
         <v>2</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="L13" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C14" s="10">
+      <c r="C14" s="7">
         <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1428,10 +1846,10 @@
       <c r="E14" s="1">
         <v>4</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="7">
         <v>3</v>
       </c>
       <c r="J14" s="2" t="s">
@@ -1440,12 +1858,12 @@
       <c r="K14" s="1">
         <v>4</v>
       </c>
-      <c r="L14" s="11" t="s">
+      <c r="L14" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C15" s="10">
+      <c r="C15" s="7">
         <v>5</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1454,10 +1872,10 @@
       <c r="E15" s="1">
         <v>6</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="7">
         <v>5</v>
       </c>
       <c r="J15" s="2" t="s">
@@ -1466,12 +1884,12 @@
       <c r="K15" s="1">
         <v>6</v>
       </c>
-      <c r="L15" s="11" t="s">
+      <c r="L15" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C16" s="10">
+      <c r="C16" s="7">
         <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1480,10 +1898,10 @@
       <c r="E16" s="1">
         <v>8</v>
       </c>
-      <c r="F16" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="10">
+      <c r="F16" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="7">
         <v>7</v>
       </c>
       <c r="J16" s="1" t="s">
@@ -1492,307 +1910,347 @@
       <c r="K16" s="1">
         <v>8</v>
       </c>
-      <c r="L16" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="13">
+      <c r="L16" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="10">
         <v>9</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="14">
+      <c r="D17" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="11">
         <v>10</v>
       </c>
-      <c r="F17" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I17" s="13">
+      <c r="F17" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="10">
         <v>9</v>
       </c>
-      <c r="J17" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="K17" s="14">
+      <c r="J17" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" s="11">
         <v>10</v>
       </c>
-      <c r="L17" s="15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C19" s="16" t="s">
+      <c r="L17" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C19" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="I19" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="16"/>
+      <c r="N19" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="O19" s="16"/>
+    </row>
+    <row r="20" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="I20" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="14"/>
+      <c r="N20" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="O20" s="14"/>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="3">
+        <v>1</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="7">
+        <v>2</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="10">
+        <v>2</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N22" s="10">
+        <v>2</v>
+      </c>
+      <c r="O22" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="7">
+        <v>3</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C24" s="7">
+        <v>4</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="16"/>
+      <c r="N24" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="O24" s="16"/>
+    </row>
+    <row r="25" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="10">
+        <v>5</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" s="14"/>
+      <c r="N25" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="O25" s="14"/>
+    </row>
+    <row r="26" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I26" s="3">
+        <v>1</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N26" s="3">
+        <v>1</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="16"/>
+      <c r="I27" s="10">
+        <v>2</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="N27" s="10">
+        <v>2</v>
+      </c>
+      <c r="O27" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="14"/>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="16"/>
+    </row>
+    <row r="30" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="7">
+        <v>2</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J30" s="14"/>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C31" s="7">
+        <v>3</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" s="3">
+        <v>1</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="7">
+        <v>4</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" s="10">
+        <v>2</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="10">
+        <v>5</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I34" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J34" s="16"/>
+    </row>
+    <row r="35" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="I19" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="17"/>
-    </row>
-    <row r="20" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="18" t="s">
+      <c r="D35" s="16"/>
+      <c r="I35" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J35" s="14"/>
+    </row>
+    <row r="36" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="I20" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="21"/>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C21" s="6">
-        <v>1</v>
-      </c>
-      <c r="D21" s="9" t="s">
+      <c r="D36" s="21"/>
+      <c r="I36" s="3">
+        <v>1</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C37" s="3">
+        <v>1</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I21" s="6">
-        <v>1</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="10">
+      <c r="I37" s="7">
         <v>2</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="J37" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="7">
+        <v>2</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I38" s="10">
+        <v>3</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C39" s="7">
+        <v>3</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="10">
+        <v>4</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J40" s="16"/>
+    </row>
+    <row r="41" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I41" s="13"/>
+      <c r="J41" s="14"/>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="I42" s="3">
+        <v>1</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I43" s="10">
         <v>2</v>
       </c>
-      <c r="J22" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="10">
-        <v>3</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="13">
-        <v>4</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I24" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="J24" s="17"/>
-    </row>
-    <row r="25" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I25" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J25" s="21"/>
-    </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C26" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="17"/>
-      <c r="I26" s="6">
-        <v>1</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C27" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="21"/>
-      <c r="I27" s="13">
-        <v>2</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="6">
-        <v>1</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C29" s="10">
-        <v>2</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I29" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="J29" s="17"/>
-    </row>
-    <row r="30" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="10">
-        <v>3</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I30" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J30" s="21"/>
-    </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C31" s="10">
-        <v>4</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I31" s="6">
-        <v>1</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="13">
-        <v>5</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I32" s="13">
-        <v>2</v>
-      </c>
-      <c r="J32" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C34" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="17"/>
-      <c r="I34" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J34" s="17"/>
-    </row>
-    <row r="35" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C35" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="21"/>
-      <c r="I35" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J35" s="21"/>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C36" s="6">
-        <v>1</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I36" s="6">
-        <v>1</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C37" s="10">
-        <v>2</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I37" s="10">
-        <v>2</v>
-      </c>
-      <c r="J37" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C38" s="10">
-        <v>3</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I38" s="13">
-        <v>3</v>
-      </c>
-      <c r="J38" s="15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="10">
-        <v>4</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C40" s="13">
-        <v>5</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I40" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="J40" s="17"/>
-    </row>
-    <row r="41" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I41" s="20"/>
-      <c r="J41" s="21"/>
-    </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="I42" s="6">
-        <v>1</v>
-      </c>
-      <c r="J42" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="3:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I43" s="13">
-        <v>2</v>
-      </c>
-      <c r="J43" s="15" t="s">
+      <c r="J43" s="12" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
+  <mergeCells count="24">
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="I5:L5"/>
     <mergeCell ref="I12:L12"/>
     <mergeCell ref="I19:J19"/>
@@ -1802,10 +2260,15 @@
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I41:J41"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>